<commit_message>
Massa de dados e prints
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_BDD/AdvantageBDDUtil/Cadastro.xlsx
+++ b/src/main/java/br/com/rsinet/hub_BDD/AdvantageBDDUtil/Cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehaime.silva\Documents\projeto\WorkSpace\AdvantageBDDTest\WorkSpace\AdvantageBDD\src\main\java\br\com\rsinet\hub_BDD\AdvantageBDDUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD49A9F-7377-4222-A347-11BBA77BD576}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D46D77-CE99-4B5A-B225-BDBCC9BA4BFD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{2EC8C595-F690-4BCD-8654-8D49096B86F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2EC8C595-F690-4BCD-8654-8D49096B86F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -81,25 +81,25 @@
     <t>Osasco</t>
   </si>
   <si>
-    <t>Brasil</t>
-  </si>
-  <si>
     <t>03454-230</t>
   </si>
   <si>
     <t>selecionaPais</t>
   </si>
   <si>
-    <t>Denmark</t>
-  </si>
-  <si>
     <t>(11) 943257234</t>
   </si>
   <si>
-    <t>Gehaime94945</t>
-  </si>
-  <si>
     <t>StarTrek234</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Gehaime8494949</t>
+  </si>
+  <si>
+    <t>bolivia</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:BR18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -878,16 +878,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -912,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:70" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>